<commit_message>
added reflection and changed coding and test cases
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayanhaq/PycharmProjects/cs151-lab7-laure_rayan_lab7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timeg_5sap6w9\PycharmProjects\cs151-lab7-laure_rayan_lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD274CB3-EB22-6D4A-978E-7FA0F8AA623B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A088D4-E04E-422B-98A1-BB8D88602066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7480" yWindow="800" windowWidth="29400" windowHeight="16660" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>&lt;-- final overall cost</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>tyle</t>
+  </si>
+  <si>
+    <t>tile</t>
   </si>
 </sst>
 </file>
@@ -581,20 +584,20 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="23.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
@@ -609,7 +612,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -630,7 +633,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -652,7 +655,7 @@
         <v>3.99</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -674,7 +677,7 @@
         <v>4.99</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -690,7 +693,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -706,9 +709,9 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>9</v>
@@ -722,7 +725,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>

</xml_diff>